<commit_message>
Excel Recap and Exception Intro
</commit_message>
<xml_diff>
--- a/testdata/Test.xlsx
+++ b/testdata/Test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syntax/eclipse-workspace/JavaBasics/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1314E2-485F-5A46-8EEB-D7D1D5645AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E04915-49F5-1648-96B2-B3EE74031274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="460" windowWidth="25580" windowHeight="15540" xr2:uid="{DD6EF329-E704-714F-A2DA-2F95175D7E30}"/>
+    <workbookView xWindow="36480" yWindow="460" windowWidth="25580" windowHeight="15540" activeTab="2" xr2:uid="{DD6EF329-E704-714F-A2DA-2F95175D7E30}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="TestData" sheetId="1" r:id="rId3"/>
     <sheet name="TestSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -435,75 +435,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7002651F-DBA2-0840-887B-D582273FA891}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="34" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="16384" width="21.5" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>20151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1">
-        <v>12345</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C12F92C-6800-D54E-A556-E99427720B37}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -517,7 +448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55FD92E-A9DD-B34A-AA93-490B1C1CB95E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -525,6 +456,75 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7002651F-DBA2-0840-887B-D582273FA891}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="34" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="21.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>